<commit_message>
update undergrad coursework spreadsheet
</commit_message>
<xml_diff>
--- a/coursework.xlsx
+++ b/coursework.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10814"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/derekhancock/Documents/online_portfolio/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/derekhancock/Documents/projects/dereklh4.github.io/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFB6A73C-5DAD-7A41-AB90-3D79F83C2511}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25600" yWindow="460" windowWidth="38400" windowHeight="21140" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14640" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150000"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -173,7 +174,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -214,6 +215,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -481,11 +485,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C32"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A3:C34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -494,42 +498,20 @@
     <col min="3" max="3" width="28.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
-    </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>16</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B4" t="s">
         <v>3</v>
@@ -540,168 +522,174 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B6" t="s">
         <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>27</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B7" t="s">
-        <v>3</v>
+        <v>19</v>
+      </c>
+      <c r="C7" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B8" t="s">
         <v>3</v>
       </c>
       <c r="C8" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B9" t="s">
         <v>3</v>
-      </c>
-      <c r="C9" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B10" t="s">
         <v>3</v>
       </c>
       <c r="C10" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="B11" t="s">
         <v>3</v>
       </c>
       <c r="C11" t="s">
-        <v>46</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B12" t="s">
         <v>3</v>
       </c>
       <c r="C12" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B13" t="s">
         <v>3</v>
       </c>
       <c r="C13" t="s">
-        <v>35</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B14" t="s">
         <v>3</v>
       </c>
       <c r="C14" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B15" t="s">
         <v>3</v>
       </c>
       <c r="C15" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>38</v>
+      </c>
+      <c r="B17" t="s">
+        <v>3</v>
+      </c>
+      <c r="C17" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
         <v>33</v>
       </c>
-      <c r="B16" t="s">
-        <v>3</v>
-      </c>
-      <c r="C16" t="s">
+      <c r="B18" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18" t="s">
         <v>35</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>0</v>
-      </c>
-      <c r="B20" t="s">
-        <v>1</v>
-      </c>
-      <c r="C20" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>8</v>
-      </c>
-      <c r="B21" t="s">
-        <v>3</v>
+        <v>43</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="B22" t="s">
-        <v>3</v>
+        <v>1</v>
+      </c>
+      <c r="C22" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>29</v>
+        <v>8</v>
       </c>
       <c r="B23" t="s">
         <v>3</v>
@@ -709,56 +697,53 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>7</v>
+        <v>30</v>
       </c>
       <c r="B24" t="s">
         <v>3</v>
-      </c>
-      <c r="C24" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="B25" t="s">
         <v>3</v>
-      </c>
-      <c r="C25" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B26" t="s">
         <v>3</v>
+      </c>
+      <c r="C26" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>42</v>
+        <v>13</v>
       </c>
       <c r="B27" t="s">
         <v>3</v>
+      </c>
+      <c r="C27" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B28" t="s">
-        <v>10</v>
-      </c>
-      <c r="C28" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>12</v>
+        <v>42</v>
       </c>
       <c r="B29" t="s">
         <v>3</v>
@@ -766,15 +751,18 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>40</v>
+        <v>9</v>
       </c>
       <c r="B30" t="s">
-        <v>3</v>
+        <v>10</v>
+      </c>
+      <c r="C30" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>39</v>
+        <v>12</v>
       </c>
       <c r="B31" t="s">
         <v>3</v>
@@ -782,9 +770,25 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
+        <v>40</v>
+      </c>
+      <c r="B32" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>39</v>
+      </c>
+      <c r="B33" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
         <v>41</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B34" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>